<commit_message>
Update University spaces data.xlsx
</commit_message>
<xml_diff>
--- a/University spaces data.xlsx
+++ b/University spaces data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mythriambatipudi/Documents/ES 96/RiskAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B46DF9D-A2C0-6B4C-B49C-F70F0F64B921}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F26E5C1-1A9B-0541-8049-8677B84B39A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16460" xr2:uid="{44193B54-3E61-4F42-A2F5-334423EA9A74}"/>
   </bookViews>
@@ -272,7 +272,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="173" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -445,18 +445,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -478,6 +469,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76E7E890-1B38-6B42-99DB-B4356D4A93F6}">
   <dimension ref="A1:K162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+    <sheetView tabSelected="1" topLeftCell="E22" workbookViewId="0">
+      <selection activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -817,50 +817,50 @@
     <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="14" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:11" s="11" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="18"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="15"/>
     </row>
     <row r="3" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
     </row>
     <row r="5" spans="1:11" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -880,7 +880,7 @@
       <c r="B8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="10">
         <v>1E-3</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -889,7 +889,7 @@
       <c r="F8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="10">
         <v>1E-3</v>
       </c>
       <c r="I8" s="1" t="s">
@@ -898,7 +898,7 @@
       <c r="J8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8" s="10">
         <v>1E-3</v>
       </c>
     </row>
@@ -1100,19 +1100,19 @@
       </c>
     </row>
     <row r="17" spans="1:11" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
@@ -1132,7 +1132,7 @@
       <c r="B20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="10">
         <v>1E-3</v>
       </c>
       <c r="E20" s="1" t="s">
@@ -1141,7 +1141,7 @@
       <c r="F20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G20" s="13">
+      <c r="G20" s="10">
         <v>1E-3</v>
       </c>
       <c r="I20" s="1" t="s">
@@ -1150,7 +1150,7 @@
       <c r="J20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K20" s="13">
+      <c r="K20" s="10">
         <v>1E-3</v>
       </c>
     </row>
@@ -1219,7 +1219,7 @@
       <c r="B23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C23" s="8">
         <v>3</v>
       </c>
       <c r="E23" s="1" t="s">
@@ -1228,7 +1228,7 @@
       <c r="F23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G23" s="11">
+      <c r="G23" s="8">
         <v>3</v>
       </c>
       <c r="I23" s="1" t="s">
@@ -1237,7 +1237,7 @@
       <c r="J23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K23" s="11">
+      <c r="K23" s="8">
         <v>3</v>
       </c>
     </row>
@@ -1358,19 +1358,19 @@
       </c>
     </row>
     <row r="29" spans="1:11" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
@@ -1390,7 +1390,7 @@
       <c r="B32" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="13">
+      <c r="C32" s="10">
         <v>1E-3</v>
       </c>
       <c r="E32" s="1" t="s">
@@ -1399,7 +1399,7 @@
       <c r="F32" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G32" s="13">
+      <c r="G32" s="10">
         <v>1E-3</v>
       </c>
       <c r="I32" s="1" t="s">
@@ -1408,7 +1408,7 @@
       <c r="J32" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K32" s="13">
+      <c r="K32" s="10">
         <v>1E-3</v>
       </c>
     </row>
@@ -1477,7 +1477,7 @@
       <c r="B35" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="11">
+      <c r="C35" s="8">
         <v>0.2</v>
       </c>
       <c r="E35" s="1" t="s">
@@ -1486,7 +1486,7 @@
       <c r="F35" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G35" s="11">
+      <c r="G35" s="8">
         <v>0.2</v>
       </c>
       <c r="I35" s="1" t="s">
@@ -1495,9 +1495,7 @@
       <c r="J35" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K35" s="11">
-        <v>0.2</v>
-      </c>
+      <c r="K35" s="4"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
@@ -1616,19 +1614,19 @@
       </c>
     </row>
     <row r="41" spans="1:11" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="10"/>
-      <c r="K41" s="10"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="20"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="20"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
@@ -1648,7 +1646,7 @@
       <c r="B44" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C44" s="13">
+      <c r="C44" s="10">
         <v>1E-3</v>
       </c>
       <c r="E44" s="1" t="s">
@@ -1657,7 +1655,7 @@
       <c r="F44" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G44" s="13">
+      <c r="G44" s="10">
         <v>1E-3</v>
       </c>
       <c r="I44" s="1" t="s">
@@ -1666,7 +1664,7 @@
       <c r="J44" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K44" s="13">
+      <c r="K44" s="10">
         <v>1E-3</v>
       </c>
     </row>
@@ -1735,7 +1733,7 @@
       <c r="B47" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C47" s="11">
+      <c r="C47" s="8">
         <v>0.2</v>
       </c>
       <c r="E47" s="1" t="s">
@@ -1744,7 +1742,7 @@
       <c r="F47" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G47" s="11">
+      <c r="G47" s="8">
         <v>0.2</v>
       </c>
       <c r="I47" s="1" t="s">
@@ -1753,9 +1751,7 @@
       <c r="J47" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K47" s="11">
-        <v>0.2</v>
-      </c>
+      <c r="K47" s="4"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
@@ -1885,34 +1881,34 @@
       <c r="K52" s="1"/>
     </row>
     <row r="53" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B53" s="9"/>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="9"/>
-      <c r="G53" s="9"/>
-      <c r="H53" s="9"/>
-      <c r="I53" s="9"/>
-      <c r="J53" s="9"/>
-      <c r="K53" s="9"/>
+      <c r="B53" s="22"/>
+      <c r="C53" s="22"/>
+      <c r="D53" s="22"/>
+      <c r="E53" s="22"/>
+      <c r="F53" s="22"/>
+      <c r="G53" s="22"/>
+      <c r="H53" s="22"/>
+      <c r="I53" s="22"/>
+      <c r="J53" s="22"/>
+      <c r="K53" s="22"/>
     </row>
     <row r="55" spans="1:11" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="10" t="s">
+      <c r="A55" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
-      <c r="F55" s="10"/>
-      <c r="G55" s="10"/>
-      <c r="H55" s="10"/>
-      <c r="I55" s="10"/>
-      <c r="J55" s="10"/>
-      <c r="K55" s="10"/>
+      <c r="B55" s="20"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="20"/>
+      <c r="H55" s="20"/>
+      <c r="I55" s="20"/>
+      <c r="J55" s="20"/>
+      <c r="K55" s="20"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
@@ -1929,7 +1925,7 @@
       <c r="B58" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C58" s="13">
+      <c r="C58" s="10">
         <v>1E-3</v>
       </c>
       <c r="E58" s="1" t="s">
@@ -1938,7 +1934,7 @@
       <c r="F58" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G58" s="13">
+      <c r="G58" s="10">
         <v>1E-3</v>
       </c>
     </row>
@@ -1949,14 +1945,14 @@
       <c r="B59" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C59" s="12"/>
+      <c r="C59" s="9"/>
       <c r="E59" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G59" s="12"/>
+      <c r="G59" s="9"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
@@ -1965,14 +1961,14 @@
       <c r="B60" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C60" s="12"/>
+      <c r="C60" s="9"/>
       <c r="E60" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G60" s="12"/>
+      <c r="G60" s="9"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
@@ -2071,34 +2067,34 @@
       </c>
     </row>
     <row r="67" spans="1:11" ht="26" x14ac:dyDescent="0.2">
-      <c r="A67" s="8" t="s">
+      <c r="A67" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B67" s="9"/>
-      <c r="C67" s="9"/>
-      <c r="D67" s="9"/>
-      <c r="E67" s="9"/>
-      <c r="F67" s="9"/>
-      <c r="G67" s="9"/>
-      <c r="H67" s="9"/>
-      <c r="I67" s="9"/>
-      <c r="J67" s="9"/>
-      <c r="K67" s="9"/>
+      <c r="B67" s="22"/>
+      <c r="C67" s="22"/>
+      <c r="D67" s="22"/>
+      <c r="E67" s="22"/>
+      <c r="F67" s="22"/>
+      <c r="G67" s="22"/>
+      <c r="H67" s="22"/>
+      <c r="I67" s="22"/>
+      <c r="J67" s="22"/>
+      <c r="K67" s="22"/>
     </row>
     <row r="69" spans="1:11" ht="21" x14ac:dyDescent="0.2">
-      <c r="A69" s="10" t="s">
+      <c r="A69" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B69" s="10"/>
-      <c r="C69" s="10"/>
-      <c r="D69" s="10"/>
-      <c r="E69" s="10"/>
-      <c r="F69" s="10"/>
-      <c r="G69" s="10"/>
-      <c r="H69" s="10"/>
-      <c r="I69" s="10"/>
-      <c r="J69" s="10"/>
-      <c r="K69" s="10"/>
+      <c r="B69" s="20"/>
+      <c r="C69" s="20"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="20"/>
+      <c r="F69" s="20"/>
+      <c r="G69" s="20"/>
+      <c r="H69" s="20"/>
+      <c r="I69" s="20"/>
+      <c r="J69" s="20"/>
+      <c r="K69" s="20"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
@@ -2115,7 +2111,7 @@
       <c r="B72" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C72" s="13">
+      <c r="C72" s="10">
         <v>1E-3</v>
       </c>
       <c r="E72" s="1" t="s">
@@ -2124,7 +2120,7 @@
       <c r="F72" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G72" s="13">
+      <c r="G72" s="10">
         <v>1E-3</v>
       </c>
     </row>
@@ -2135,7 +2131,7 @@
       <c r="B73" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C73" s="15">
+      <c r="C73" s="12">
         <v>135</v>
       </c>
       <c r="E73" s="1" t="s">
@@ -2144,7 +2140,7 @@
       <c r="F73" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G73" s="15">
+      <c r="G73" s="12">
         <v>54</v>
       </c>
     </row>
@@ -2184,7 +2180,7 @@
       <c r="F75" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G75" s="11">
+      <c r="G75" s="8">
         <v>2.5</v>
       </c>
     </row>
@@ -2269,19 +2265,19 @@
       </c>
     </row>
     <row r="81" spans="1:11" ht="21" x14ac:dyDescent="0.2">
-      <c r="A81" s="10" t="s">
+      <c r="A81" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B81" s="10"/>
-      <c r="C81" s="10"/>
-      <c r="D81" s="10"/>
-      <c r="E81" s="10"/>
-      <c r="F81" s="10"/>
-      <c r="G81" s="10"/>
-      <c r="H81" s="10"/>
-      <c r="I81" s="10"/>
-      <c r="J81" s="10"/>
-      <c r="K81" s="10"/>
+      <c r="B81" s="20"/>
+      <c r="C81" s="20"/>
+      <c r="D81" s="20"/>
+      <c r="E81" s="20"/>
+      <c r="F81" s="20"/>
+      <c r="G81" s="20"/>
+      <c r="H81" s="20"/>
+      <c r="I81" s="20"/>
+      <c r="J81" s="20"/>
+      <c r="K81" s="20"/>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
@@ -2296,12 +2292,12 @@
       <c r="B84" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C84" s="13">
+      <c r="C84" s="10">
         <v>1E-3</v>
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
-      <c r="G84" s="13"/>
+      <c r="G84" s="10"/>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
@@ -2310,12 +2306,12 @@
       <c r="B85" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C85" s="15">
+      <c r="C85" s="12">
         <v>16</v>
       </c>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
-      <c r="G85" s="15"/>
+      <c r="G85" s="12"/>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
@@ -2343,7 +2339,7 @@
       </c>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
-      <c r="G87" s="11"/>
+      <c r="G87" s="8"/>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
@@ -2402,19 +2398,19 @@
       <c r="G91" s="1"/>
     </row>
     <row r="93" spans="1:11" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="10" t="s">
+      <c r="A93" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B93" s="10"/>
-      <c r="C93" s="10"/>
-      <c r="D93" s="10"/>
-      <c r="E93" s="10"/>
-      <c r="F93" s="10"/>
-      <c r="G93" s="10"/>
-      <c r="H93" s="10"/>
-      <c r="I93" s="10"/>
-      <c r="J93" s="10"/>
-      <c r="K93" s="10"/>
+      <c r="B93" s="20"/>
+      <c r="C93" s="20"/>
+      <c r="D93" s="20"/>
+      <c r="E93" s="20"/>
+      <c r="F93" s="20"/>
+      <c r="G93" s="20"/>
+      <c r="H93" s="20"/>
+      <c r="I93" s="20"/>
+      <c r="J93" s="20"/>
+      <c r="K93" s="20"/>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
@@ -2434,7 +2430,7 @@
       <c r="B96" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C96" s="13">
+      <c r="C96" s="10">
         <v>1E-3</v>
       </c>
       <c r="E96" s="1" t="s">
@@ -2443,7 +2439,7 @@
       <c r="F96" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G96" s="13">
+      <c r="G96" s="10">
         <v>1E-3</v>
       </c>
       <c r="I96" s="1" t="s">
@@ -2452,7 +2448,7 @@
       <c r="J96" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K96" s="13">
+      <c r="K96" s="10">
         <v>1E-3</v>
       </c>
     </row>
@@ -2521,7 +2517,7 @@
       <c r="B99" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C99" s="11">
+      <c r="C99" s="8">
         <v>0.4</v>
       </c>
       <c r="E99" s="1" t="s">
@@ -2530,7 +2526,7 @@
       <c r="F99" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G99" s="11">
+      <c r="G99" s="8">
         <v>0.4</v>
       </c>
       <c r="I99" s="1" t="s">
@@ -2539,7 +2535,7 @@
       <c r="J99" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K99" s="11">
+      <c r="K99" s="8">
         <v>0.1</v>
       </c>
     </row>
@@ -2660,19 +2656,19 @@
       </c>
     </row>
     <row r="105" spans="1:11" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="10" t="s">
+      <c r="A105" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B105" s="10"/>
-      <c r="C105" s="10"/>
-      <c r="D105" s="10"/>
-      <c r="E105" s="10"/>
-      <c r="F105" s="10"/>
-      <c r="G105" s="10"/>
-      <c r="H105" s="10"/>
-      <c r="I105" s="10"/>
-      <c r="J105" s="10"/>
-      <c r="K105" s="10"/>
+      <c r="B105" s="20"/>
+      <c r="C105" s="20"/>
+      <c r="D105" s="20"/>
+      <c r="E105" s="20"/>
+      <c r="F105" s="20"/>
+      <c r="G105" s="20"/>
+      <c r="H105" s="20"/>
+      <c r="I105" s="20"/>
+      <c r="J105" s="20"/>
+      <c r="K105" s="20"/>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
@@ -2692,7 +2688,7 @@
       <c r="B108" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C108" s="13">
+      <c r="C108" s="10">
         <v>1E-3</v>
       </c>
       <c r="E108" s="1" t="s">
@@ -2701,7 +2697,7 @@
       <c r="F108" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G108" s="13">
+      <c r="G108" s="10">
         <v>1E-3</v>
       </c>
       <c r="I108" s="1" t="s">
@@ -2710,7 +2706,7 @@
       <c r="J108" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K108" s="13">
+      <c r="K108" s="10">
         <v>1E-3</v>
       </c>
     </row>
@@ -2779,7 +2775,7 @@
       <c r="B111" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C111" s="11">
+      <c r="C111" s="8">
         <v>0.4</v>
       </c>
       <c r="E111" s="1" t="s">
@@ -2788,7 +2784,7 @@
       <c r="F111" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G111" s="11">
+      <c r="G111" s="8">
         <v>0.4</v>
       </c>
       <c r="I111" s="1" t="s">
@@ -2797,7 +2793,7 @@
       <c r="J111" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K111" s="11">
+      <c r="K111" s="8">
         <v>0.1</v>
       </c>
     </row>
@@ -2918,34 +2914,34 @@
       </c>
     </row>
     <row r="117" spans="1:11" ht="26" x14ac:dyDescent="0.2">
-      <c r="A117" s="8" t="s">
+      <c r="A117" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B117" s="9"/>
-      <c r="C117" s="9"/>
-      <c r="D117" s="9"/>
-      <c r="E117" s="9"/>
-      <c r="F117" s="9"/>
-      <c r="G117" s="9"/>
-      <c r="H117" s="9"/>
-      <c r="I117" s="9"/>
-      <c r="J117" s="9"/>
-      <c r="K117" s="9"/>
+      <c r="B117" s="22"/>
+      <c r="C117" s="22"/>
+      <c r="D117" s="22"/>
+      <c r="E117" s="22"/>
+      <c r="F117" s="22"/>
+      <c r="G117" s="22"/>
+      <c r="H117" s="22"/>
+      <c r="I117" s="22"/>
+      <c r="J117" s="22"/>
+      <c r="K117" s="22"/>
     </row>
     <row r="119" spans="1:11" ht="21" x14ac:dyDescent="0.2">
-      <c r="A119" s="10" t="s">
+      <c r="A119" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B119" s="10"/>
-      <c r="C119" s="10"/>
-      <c r="D119" s="10"/>
-      <c r="E119" s="10"/>
-      <c r="F119" s="10"/>
-      <c r="G119" s="10"/>
-      <c r="H119" s="10"/>
-      <c r="I119" s="10"/>
-      <c r="J119" s="10"/>
-      <c r="K119" s="10"/>
+      <c r="B119" s="20"/>
+      <c r="C119" s="20"/>
+      <c r="D119" s="20"/>
+      <c r="E119" s="20"/>
+      <c r="F119" s="20"/>
+      <c r="G119" s="20"/>
+      <c r="H119" s="20"/>
+      <c r="I119" s="20"/>
+      <c r="J119" s="20"/>
+      <c r="K119" s="20"/>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
@@ -2954,7 +2950,7 @@
       <c r="B120" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C120" s="13">
+      <c r="C120" s="10">
         <v>1E-3</v>
       </c>
     </row>
@@ -2998,7 +2994,7 @@
       <c r="B124" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C124" s="11">
+      <c r="C124" s="8">
         <v>3</v>
       </c>
     </row>
@@ -3047,49 +3043,49 @@
       </c>
     </row>
     <row r="130" spans="1:11" ht="21" x14ac:dyDescent="0.2">
-      <c r="A130" s="10" t="s">
+      <c r="A130" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B130" s="10"/>
-      <c r="C130" s="10"/>
-      <c r="D130" s="10"/>
-      <c r="E130" s="10"/>
-      <c r="F130" s="10"/>
-      <c r="G130" s="10"/>
-      <c r="H130" s="10"/>
-      <c r="I130" s="10"/>
-      <c r="J130" s="10"/>
-      <c r="K130" s="10"/>
-    </row>
-    <row r="131" spans="1:11" s="20" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="19"/>
-      <c r="B131" s="19"/>
-      <c r="C131" s="19"/>
-      <c r="D131" s="19"/>
-      <c r="E131" s="19"/>
-      <c r="F131" s="19"/>
-      <c r="G131" s="19"/>
-      <c r="H131" s="19"/>
-      <c r="I131" s="19"/>
-      <c r="J131" s="19"/>
-      <c r="K131" s="19"/>
-    </row>
-    <row r="132" spans="1:11" s="20" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="21" t="s">
+      <c r="B130" s="20"/>
+      <c r="C130" s="20"/>
+      <c r="D130" s="20"/>
+      <c r="E130" s="20"/>
+      <c r="F130" s="20"/>
+      <c r="G130" s="20"/>
+      <c r="H130" s="20"/>
+      <c r="I130" s="20"/>
+      <c r="J130" s="20"/>
+      <c r="K130" s="20"/>
+    </row>
+    <row r="131" spans="1:11" s="17" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="16"/>
+      <c r="B131" s="16"/>
+      <c r="C131" s="16"/>
+      <c r="D131" s="16"/>
+      <c r="E131" s="16"/>
+      <c r="F131" s="16"/>
+      <c r="G131" s="16"/>
+      <c r="H131" s="16"/>
+      <c r="I131" s="16"/>
+      <c r="J131" s="16"/>
+      <c r="K131" s="16"/>
+    </row>
+    <row r="132" spans="1:11" s="17" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="B132" s="19"/>
-      <c r="C132" s="19"/>
-      <c r="D132" s="19"/>
-      <c r="E132" s="21" t="s">
+      <c r="B132" s="16"/>
+      <c r="C132" s="16"/>
+      <c r="D132" s="16"/>
+      <c r="E132" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="F132" s="19"/>
-      <c r="G132" s="19"/>
-      <c r="H132" s="19"/>
-      <c r="I132" s="19"/>
-      <c r="J132" s="19"/>
-      <c r="K132" s="19"/>
+      <c r="F132" s="16"/>
+      <c r="G132" s="16"/>
+      <c r="H132" s="16"/>
+      <c r="I132" s="16"/>
+      <c r="J132" s="16"/>
+      <c r="K132" s="16"/>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
@@ -3098,7 +3094,7 @@
       <c r="B133" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C133" s="13">
+      <c r="C133" s="10">
         <v>1E-3</v>
       </c>
       <c r="E133" s="1" t="s">
@@ -3107,7 +3103,7 @@
       <c r="F133" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G133" s="13">
+      <c r="G133" s="10">
         <v>1E-3</v>
       </c>
     </row>
@@ -3198,7 +3194,7 @@
       <c r="B138" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C138" s="22">
+      <c r="C138" s="19">
         <v>0.68</v>
       </c>
       <c r="E138" s="1" t="s">
@@ -3207,7 +3203,7 @@
       <c r="F138" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G138" s="22">
+      <c r="G138" s="19">
         <v>0.68</v>
       </c>
     </row>
@@ -3372,16 +3368,16 @@
       </c>
     </row>
     <row r="148" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A148" s="21" t="s">
+      <c r="A148" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="B148" s="19"/>
-      <c r="C148" s="19"/>
-      <c r="E148" s="21" t="s">
+      <c r="B148" s="16"/>
+      <c r="C148" s="16"/>
+      <c r="E148" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="F148" s="19"/>
-      <c r="G148" s="19"/>
+      <c r="F148" s="16"/>
+      <c r="G148" s="16"/>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
@@ -3390,7 +3386,7 @@
       <c r="B149" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C149" s="13">
+      <c r="C149" s="10">
         <v>1E-3</v>
       </c>
       <c r="E149" s="1" t="s">
@@ -3399,7 +3395,7 @@
       <c r="F149" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G149" s="13">
+      <c r="G149" s="10">
         <v>1E-3</v>
       </c>
     </row>
@@ -3490,7 +3486,7 @@
       <c r="B154" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C154" s="22">
+      <c r="C154" s="19">
         <v>0.68</v>
       </c>
       <c r="E154" s="1" t="s">
@@ -3499,7 +3495,7 @@
       <c r="F154" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G154" s="22">
+      <c r="G154" s="19">
         <v>0.68</v>
       </c>
     </row>
@@ -3665,6 +3661,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="A17:K17"/>
+    <mergeCell ref="A53:K53"/>
+    <mergeCell ref="A55:K55"/>
+    <mergeCell ref="A29:K29"/>
+    <mergeCell ref="A41:K41"/>
     <mergeCell ref="A119:K119"/>
     <mergeCell ref="A130:K130"/>
     <mergeCell ref="A67:K67"/>
@@ -3673,13 +3676,6 @@
     <mergeCell ref="A93:K93"/>
     <mergeCell ref="A105:K105"/>
     <mergeCell ref="A117:K117"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A17:K17"/>
-    <mergeCell ref="A53:K53"/>
-    <mergeCell ref="A55:K55"/>
-    <mergeCell ref="A29:K29"/>
-    <mergeCell ref="A41:K41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>